<commit_message>
refs #123 Spreadsheet updates for diff comparison tests.
</commit_message>
<xml_diff>
--- a/res/Test SpreadSheet.xlsx
+++ b/res/Test SpreadSheet.xlsx
@@ -73,7 +73,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -83,6 +83,7 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -316,7 +317,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2">
-        <v>2010.0</v>
+        <v>2011.0</v>
       </c>
       <c r="B2" s="2">
         <v>5.0</v>
@@ -327,7 +328,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2">
-        <v>2011.0</v>
+        <v>2012.0</v>
       </c>
       <c r="B3" s="2">
         <v>12.0</v>
@@ -338,7 +339,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2">
-        <v>2012.0</v>
+        <v>2013.0</v>
       </c>
       <c r="B4" s="2">
         <v>55.0</v>
@@ -349,7 +350,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2">
-        <v>2013.0</v>
+        <v>2014.0</v>
       </c>
       <c r="B5" s="2">
         <v>12.0</v>
@@ -360,7 +361,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2">
-        <v>2014.0</v>
+        <v>2015.0</v>
       </c>
       <c r="B6" s="2">
         <v>33.0</v>
@@ -371,7 +372,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2">
-        <v>2015.0</v>
+        <v>2016.0</v>
       </c>
       <c r="B7" s="2">
         <v>4.0</v>
@@ -382,7 +383,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2">
-        <v>2016.0</v>
+        <v>2017.0</v>
       </c>
       <c r="B8" s="2">
         <v>54.0</v>
@@ -393,7 +394,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2">
-        <v>2017.0</v>
+        <v>2018.0</v>
       </c>
       <c r="B9" s="2">
         <v>53.0</v>
@@ -404,13 +405,24 @@
     </row>
     <row r="10">
       <c r="A10" s="2">
-        <v>2018.0</v>
+        <v>2019.0</v>
       </c>
       <c r="B10" s="2">
         <v>11.0</v>
       </c>
       <c r="C10" s="2">
         <v>7.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3">
+        <f t="shared" ref="B11:C11" si="1">AVERAGE(B2:B10)</f>
+        <v>26.55555556</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>